<commit_message>
fam-seco, Frontend: Control de token y login
</commit_message>
<xml_diff>
--- a/seco-fam/doc/presupuesto.xlsx
+++ b/seco-fam/doc/presupuesto.xlsx
@@ -3,27 +3,33 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{08F8033F-E994-401F-A861-3D870C165690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE00F0-92DE-4782-80FA-6C0961E2C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cómo usar esta plantilla" sheetId="2" r:id="rId1"/>
-    <sheet name="Factura de servicio" sheetId="1" r:id="rId2"/>
+    <sheet name="GRDP001" sheetId="3" r:id="rId2"/>
+    <sheet name="GRDP002" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Nombre_de_la_compañía">'Factura de servicio'!$B$2</definedName>
-    <definedName name="RegiónDeTítuloDeColumna1..E13.1">'Factura de servicio'!#REF!</definedName>
-    <definedName name="RegiónTítuloFila1..E5">'Factura de servicio'!$D$3</definedName>
+    <definedName name="Nombre_de_la_compañía" localSheetId="1">GRDP001!$B$2</definedName>
+    <definedName name="Nombre_de_la_compañía">GRDP002!$B$2</definedName>
+    <definedName name="RegiónDeTítuloDeColumna1..E13.1" localSheetId="1">GRDP001!#REF!</definedName>
+    <definedName name="RegiónDeTítuloDeColumna1..E13.1">GRDP002!#REF!</definedName>
+    <definedName name="RegiónTítuloFila1..E5" localSheetId="1">GRDP001!$D$3</definedName>
+    <definedName name="RegiónTítuloFila1..E5">GRDP002!$D$3</definedName>
+    <definedName name="TítuloColumna1" localSheetId="1">Factura3[[#Headers],[Cantidad]]</definedName>
     <definedName name="TítuloColumna1">Factura[[#Headers],[Cantidad]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Factura de servicio'!$13:$13</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">GRDP001!$12:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">GRDP002!$13:$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Introducción al uso de la factura de servicio</t>
   </si>
@@ -196,7 +202,64 @@
     <t>IVA</t>
   </si>
   <si>
-    <t>creación UX/UI, desarrollo web, backend y frontend de una web con contraseña donde puedas descargar en formato pdf un fichero. Desde backend se tiene acceso a todos los ficheros donde sep podrán sustituir por otros.</t>
+    <t>Hosting web, correo, BBDD, certificado SSL</t>
+  </si>
+  <si>
+    <t>IP Pública fija</t>
+  </si>
+  <si>
+    <t>Tema joyería</t>
+  </si>
+  <si>
+    <t>Módulo TPV Virtual (Redsys)</t>
+  </si>
+  <si>
+    <t>Módulo SEO</t>
+  </si>
+  <si>
+    <t>Módulo Política de Cookies</t>
+  </si>
+  <si>
+    <t>Pasarela de pago con tu banco (0,2% sobre el PVP de cada producto)</t>
+  </si>
+  <si>
+    <t>Dominio (compra/renovación)</t>
+  </si>
+  <si>
+    <t>Desarrollo, Diseño web UX/UI, integración y curso de implantación</t>
+  </si>
+  <si>
+    <t>Fabio Adrián Ghibaudo</t>
+  </si>
+  <si>
+    <t>www.lavidaeshuella.es</t>
+  </si>
+  <si>
+    <t>Parque Empresarial Alvedro, Nave E 30, Manzana Nº10</t>
+  </si>
+  <si>
+    <t>15180, Alvedro (Culleredo)</t>
+  </si>
+  <si>
+    <t>981 90 90 47</t>
+  </si>
+  <si>
+    <t>23P101</t>
+  </si>
+  <si>
+    <t>GRD0001</t>
+  </si>
+  <si>
+    <t>C/ Galera nº 25, 6º</t>
+  </si>
+  <si>
+    <t>23P102</t>
+  </si>
+  <si>
+    <t>creación UX/UI, desarrollo web, backend y frontend de una web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No incluye compra de dominio, alojamiento ni integración de la aplicación </t>
   </si>
 </sst>
 </file>
@@ -210,10 +273,17 @@
     <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -702,100 +772,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" indent="9"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1">
@@ -813,89 +883,107 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="44" fontId="7" fillId="4" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="8">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" vertical="center" indent="9"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="11" applyFont="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="12" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="21" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="35" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="36" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="21" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="27" fillId="37" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="16" applyFont="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="7">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="44" fontId="1" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="11" applyFont="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="12" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="21" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="35" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="36" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="21" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="26" fillId="37" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -952,25 +1040,50 @@
     <cellStyle name="Título 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
-        <name val="Segoe UI Light"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
         <family val="2"/>
-        <scheme val="major"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="2" tint="-0.249977111117893"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="2" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="2" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1015,6 +1128,44 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1095,13 +1246,13 @@
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Factura de servicio" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="9"/>
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="totalRow" dxfId="7"/>
-      <tableStyleElement type="firstColumn" dxfId="6"/>
-      <tableStyleElement type="lastColumn" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="totalRow" dxfId="10"/>
+      <tableStyleElement type="firstColumn" dxfId="9"/>
+      <tableStyleElement type="lastColumn" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1188,6 +1339,202 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76096</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Grupo 1" descr="Borde de contenido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ED1249A-DBAA-4D62-AF0E-972E461D6E80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="838200" y="942975"/>
+          <a:ext cx="8534400" cy="2657371"/>
+          <a:chOff x="771525" y="828675"/>
+          <a:chExt cx="5766635" cy="2657371"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="Imagen 2" descr="Borde izquierdo del contenido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21EF917D-667F-4825-CEB6-D09E99FC750D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="771525" y="853670"/>
+            <a:ext cx="38095" cy="2632376"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="4" name="Imagen 3" descr="Borde derecho del contenido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{490F7519-BE0C-BC4C-569C-A92519304AC2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6500065" y="853670"/>
+            <a:ext cx="38095" cy="2632376"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Imagen 4" descr="Borde superior del contenido">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48CAB37-E7CB-78EA-8B80-B1D46D58EA5F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect t="-140025" b="-140025"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="805639" y="828675"/>
+            <a:ext cx="5702427" cy="69502"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>800012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8499C7C-7442-49BA-AE15-655EE71C2A19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047750" y="95250"/>
+          <a:ext cx="1123810" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1384,7 +1731,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Factura" displayName="Factura" ref="B13:E24" totalsRowCount="1" headerRowDxfId="0" headerRowCellStyle="Encabezado 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7A54EA12-A463-48EB-8A81-36A2106B1F8B}" name="Factura3" displayName="Factura3" ref="B12:E23" totalsRowCount="1" headerRowDxfId="4" headerRowCellStyle="Encabezado 4">
+  <autoFilter ref="B12:E22" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{965D0C2E-D7A3-43CD-BAD3-9FDE6883EEF5}" name="Cantidad"/>
+    <tableColumn id="2" xr3:uid="{92382F50-7070-433E-8576-EC3B54809EC6}" name="Descripción" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{C829CC40-5A68-4CAE-AA91-C1D1F3AB6B67}" name="Precio por unidad" totalsRowLabel="Subtotal"/>
+    <tableColumn id="5" xr3:uid="{76DF5326-18F6-4C6C-80D4-04BCF9259E7F}" name="Total de línea" totalsRowFunction="custom" totalsRowDxfId="2">
+      <calculatedColumnFormula>IFERROR(IF(SUM(B13)&gt;0,SUM(B13*D13),""), "")</calculatedColumnFormula>
+      <totalsRowFormula>IFERROR(IF(SUM(E13:E22)&gt;0,SUM(E13:E22),""), "")</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Factura de servicio" showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Escriba la cantidad, la descripción y el precio por unidad en esta tabla. El total por línea y el subtotal se calculan automáticamente."/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Factura" displayName="Factura" ref="B13:E24" totalsRowCount="1" headerRowDxfId="5" headerRowCellStyle="Encabezado 4">
   <autoFilter ref="B13:E23" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1393,9 +1766,9 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Cantidad"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción" totalsRowDxfId="1"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Precio por unidad" totalsRowLabel="Subtotal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total de línea" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total de línea" totalsRowFunction="custom" totalsRowDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(SUM(B14)&gt;0,SUM(B14*D14),""), "")</calculatedColumnFormula>
       <totalsRowFormula>IFERROR(IF(SUM(E14:E23)&gt;0,SUM(E14:E23),""), "")</totalsRowFormula>
     </tableColumn>
@@ -1686,6 +2059,388 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C80EEAF-80EA-48A8-8AC7-47AD5422A80A}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:E28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="2.625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45082</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="41"/>
+    </row>
+    <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="37">
+        <v>191.88</v>
+      </c>
+      <c r="E13" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>191.88</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="39">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="38">
+        <v>20</v>
+      </c>
+      <c r="E14" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="37">
+        <v>11.95</v>
+      </c>
+      <c r="E15" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="39">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="38">
+        <v>120</v>
+      </c>
+      <c r="E16" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="37">
+        <v>70</v>
+      </c>
+      <c r="E17" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="39">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="38">
+        <v>200</v>
+      </c>
+      <c r="E18" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="37">
+        <v>70</v>
+      </c>
+      <c r="E19" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="39">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="38">
+        <v>1400</v>
+      </c>
+      <c r="E20" s="28">
+        <f>Factura3[[#This Row],[Precio por unidad]]*Factura3[[#This Row],[Cantidad]]</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="29">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21">
+        <f t="shared" ref="E21:E22" si="0">IFERROR(IF(SUM(B21)&gt;0,SUM(B21*D21),""), "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="23"/>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="36">
+        <f>IFERROR(IF(SUM(E13:E22)&gt;0,SUM(E13:E22),""), "")</f>
+        <v>2083.83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="E24" s="26">
+        <f>IFERROR(IF(SUM(Factura3[[#Totals],[Total de línea]])&gt;0,SUM(Factura3[[#Totals],[Total de línea]]*D24),""), "")</f>
+        <v>437.60429999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="27">
+        <f>IFERROR(IF(SUM(Factura3[[#Totals],[Total de línea]])&gt;0,SUM(Factura3[[#Totals],[Total de línea]],E24),""), "")</f>
+        <v>2521.4342999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="35" t="str">
+        <f>"Presupuesto válido durante 3 meses desde el envío de este documento."</f>
+        <v>Presupuesto válido durante 3 meses desde el envío de este documento.</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+    </row>
+    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <dataValidations count="30">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la tasa de impuesto sobre las ventas en la celda de la derecha." sqref="B24:C24" xr:uid="{33980E37-FAAC-4E99-8B6A-AA7B8B497E6C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Agregue el logotipo de la compañía en esta celda, el eslogan en la celda de la derecha y el nombre, la dirección, la ciudad, el estado, el código postal, el número de teléfono, el de fax y la dirección de correo electrónico en las celdas siguientes." sqref="B1" xr:uid="{9E5F73A2-691D-47FB-9ABB-B3A49E5EA1D6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El total se calcula automáticamente en esta celda." sqref="E25:E26" xr:uid="{61F546A1-5F0F-4F65-8A02-EC3DF80FDB7B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El importe de Impuesto sobre las ventas se calcula automáticamente en esta celda con el porcentaje del impuesto sobre las ventas de la celda de la izquierda." sqref="E24" xr:uid="{2E991E6E-D9DD-4B83-9FDF-CA45E5766EDD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cree una factura de servicio en esta hoja de cálculo siguiendo las instrucciones que se proporcionan en Cómo usar esta hoja de cálculo de plantilla. Agregue el logotipo de la compañía en la celda de la derecha." sqref="A1" xr:uid="{22153248-4FC4-4981-8CDF-0CC1C706F8F4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El total se calcula automáticamente en la celda derecha." sqref="B25:D26" xr:uid="{0A8F34BA-A3C3-4589-B6BC-E73E7E2AC44B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la tasa de impuesto sobre las ventas en esta celda. El importe del impuesto se calcula automáticamente en la celda de la derecha." sqref="D24" xr:uid="{F8C6EF2C-7647-4CDA-9F23-3484C03573A5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El valor de Total de línea se calcula automáticamente en esta columna debajo de este encabezado." sqref="E12" xr:uid="{B6D399C2-1DC2-466F-90B8-0873769E8D2E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el precio unitario en esta columna debajo de este encabezado." sqref="D12" xr:uid="{8AC2BEDC-D33C-4E1B-95A6-C44B066517EA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la descripción en esta columna debajo de este encabezado." sqref="C12" xr:uid="{4E578068-5C4D-4C11-A662-30D453DF8F1B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la cantidad en la columna debajo de este encabezado." sqref="B12" xr:uid="{B6295814-0038-46C7-841C-22BA46989BAF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el número de teléfono del cliente en esta celda." sqref="B11:C11" xr:uid="{F2EFBCE7-A0CB-4D94-9834-D6DF34B2F215}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la ciudad, el estado y el código postal del cliente en esta celda." sqref="B10:C10" xr:uid="{6516381B-FC99-4372-9C2F-BEEB0CFB0189}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la dirección del cliente en esta celda." sqref="B9:C9" xr:uid="{DAD6AF99-6042-465F-8AC9-311F1F10AB20}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el nombre de la empresa en esta celda." sqref="B8:C8" xr:uid="{42407BD1-8EA6-40B8-95E1-EAF485C068C1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el nombre del cliente en esta celda." sqref="B7:C7" xr:uid="{AA5EAB15-3FFD-4815-B01E-67A7FA5BA422}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el Id. del cliente en esta celda." sqref="E5" xr:uid="{6C78CEB7-A2C5-4FE0-B95C-82BF0D23C23A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el id. del cliente en la celda de la derecha." sqref="D5" xr:uid="{568B5E8F-D258-444D-B0C8-052D52637D28}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la fecha de la factura en esta celda." sqref="E4" xr:uid="{745415B6-DE75-4298-9ECB-AE3F48F97613}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la fecha de la factura en la celda de la derecha." sqref="D4" xr:uid="{C6017023-9999-43F0-B40C-AEB8D94976DB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el número de factura en esta celda." sqref="E3" xr:uid="{D14CA629-9BBD-41E5-BCB8-CD71D54E36BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el número de factura en la celda de la derecha." sqref="D3" xr:uid="{D5155169-D32F-4614-A19E-CB5C05275964}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la dirección de correo electrónico en esta celda." sqref="B6" xr:uid="{4F11D459-56DF-4DE8-9DD5-B61E10A2923A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba los números de teléfono y fax entre corchetes en esta celda." sqref="B5:C5" xr:uid="{C23A4A02-7101-4AA3-A36C-F8F3BFDCCA08}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la ciudad, el estado y el código postal en esta celda." sqref="B4:C4" xr:uid="{A7E959F4-2B42-4216-AFF6-A8DCB7019D7D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba la dirección de la empresa de facturación en esta celda." sqref="B3:C3" xr:uid="{BF005AAB-4E81-4B8A-A50D-CDE255FF218E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el nombre de la compañía de facturación en esta celda." sqref="B2" xr:uid="{B560B266-4DD6-4310-A7E5-A5F5F8FF815E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El título de esta hoja de cálculo se encuentra en esta celda. Escriba el número de factura, la fecha de la factura y el Id. de cliente en las celdas comprendidas entre la D3 y la E5." sqref="D1:E1" xr:uid="{2B929DC6-D2E2-4CFE-83EC-DAEA63003361}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el eslogan de la compañía en esta celda." sqref="C1" xr:uid="{E7E18EB6-AAC6-42A2-9407-B4F3BBA2ABC9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El nombre de la compañía se anexa automáticamente en esta celda." sqref="B27:E27" xr:uid="{D2EA6AA2-2046-441C-A67A-F8FFE60BEA1C}"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{0F7A749A-5C49-45E0-8C29-55C826CCC6DC}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{1F35DB61-CE7B-4F88-8298-390AF76EB01B}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.51181102362204722" bottom="0.51181102362204722" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <headerFooter differentFirst="1">
+    <oddHeader>&amp;L&amp;G</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="E13:E20" calculatedColumn="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId4"/>
+  <legacyDrawingHF r:id="rId5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
@@ -1694,7 +2449,7 @@
   <dimension ref="B1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1711,13 +2466,13 @@
     <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="22"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1"/>
@@ -1725,18 +2480,18 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3">
-        <v>23100</v>
+      <c r="E3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="12"/>
@@ -1745,11 +2500,11 @@
       </c>
       <c r="E4" s="3">
         <f ca="1">TODAY()</f>
-        <v>45085</v>
+        <v>45086</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="10"/>
@@ -1761,7 +2516,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1794,47 +2549,50 @@
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="66" x14ac:dyDescent="0.3">
-      <c r="B14" s="33">
+    <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="29">
         <v>1</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="32">
+      <c r="C14" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="28">
         <v>300</v>
       </c>
-      <c r="E14" s="25">
-        <v>250</v>
+      <c r="E14" s="28">
+        <f>Factura[[#This Row],[Precio por unidad]]*Factura[[#This Row],[Cantidad]]</f>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7" t="str">
-        <f t="shared" ref="E14:E23" si="0">IFERROR(IF(SUM(B15)&gt;0,SUM(B15*D15),""), "")</f>
+        <f t="shared" ref="E15:E23" si="0">IFERROR(IF(SUM(B15)&gt;0,SUM(B15*D15),""), "")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="str">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1851,10 +2609,10 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="str">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1869,10 +2627,10 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="str">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1887,44 +2645,44 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25" t="str">
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="28"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="27"/>
+      <c r="C24" s="23"/>
       <c r="D24" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="25">
         <f>IFERROR(IF(SUM(E14:E23)&gt;0,SUM(E14:E23),""), "")</f>
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="5">
         <v>0.21</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="26">
         <f>IFERROR(IF(SUM(Factura[[#Totals],[Total de línea]])&gt;0,SUM(Factura[[#Totals],[Total de línea]]*D25),""), "")</f>
-        <v>52.5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1933,9 +2691,9 @@
       <c r="D26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="27">
         <f>IFERROR(IF(SUM(Factura[[#Totals],[Total de línea]])&gt;0,SUM(Factura[[#Totals],[Total de línea]],E25),""), "")</f>
-        <v>302.5</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1945,21 +2703,21 @@
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="str">
+      <c r="B28" s="35" t="str">
         <f>"Presupuesto válido durante 3 meses desde el envío de este documento."</f>
         <v>Presupuesto válido durante 3 meses desde el envío de este documento.</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1968,7 +2726,7 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B28:E28"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="30">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="El nombre de la compañía se anexa automáticamente en esta celda." sqref="B28:E28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Escriba el eslogan de la compañía en esta celda." sqref="C1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
@@ -2013,7 +2771,6 @@
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="E15:E23" emptyCellReference="1"/>
-    <ignoredError sqref="E14" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawingHF r:id="rId4"/>
@@ -2024,6 +2781,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2311,36 +3097,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{673FC2C4-7BD3-49D4-8830-2C75FF0E170D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEA9B86-3ACC-4F2F-B417-3306CFE473B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33998CD7-F07C-4773-9B85-057C9552A5A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2359,24 +3136,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEA9B86-3ACC-4F2F-B417-3306CFE473B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{673FC2C4-7BD3-49D4-8830-2C75FF0E170D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
seco-fam, Frontend: control del token
</commit_message>
<xml_diff>
--- a/seco-fam/doc/presupuesto.xlsx
+++ b/seco-fam/doc/presupuesto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE00F0-92DE-4782-80FA-6C0961E2C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B33155-07E0-4207-9D46-D5CA6991130C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cómo usar esta plantilla" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Introducción al uso de la factura de servicio</t>
   </si>
@@ -130,18 +130,6 @@
     <t>Escriba el número de factura y el Id. de cliente. La fecha se rellena automáticamente. Después, escriba la información del cliente: nombre de contacto, nombre de la compañía, dirección y teléfono. Defina la tasa de impuesto en la celda D27. El nombre de la compañía se anexa automáticamente en la celda B29. Por último, escriba toda la información de la transacción del pedido en la tabla Factura a partir de la celda B15.</t>
   </si>
   <si>
-    <t>Dirección</t>
-  </si>
-  <si>
-    <t>Ciudad y código postal</t>
-  </si>
-  <si>
-    <t>Nombre de la empresa</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
     <t>Cantidad</t>
   </si>
   <si>
@@ -260,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">No incluye compra de dominio, alojamiento ni integración de la aplicación </t>
+  </si>
+  <si>
+    <t>Rúa Casares Quiroga, 49</t>
+  </si>
+  <si>
+    <t>15179, Oleiros</t>
   </si>
 </sst>
 </file>
@@ -955,32 +949,32 @@
     <xf numFmtId="44" fontId="27" fillId="37" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="1" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="16" applyFont="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="16" applyFont="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="5" borderId="0" xfId="21" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1087,6 +1081,25 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Segoe UI Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1128,25 +1141,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Segoe UI Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1544,8 +1538,8 @@
       <xdr:rowOff>828675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>380896</xdr:rowOff>
     </xdr:to>
@@ -1685,8 +1679,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>152260</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257160</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>800012</xdr:rowOff>
     </xdr:to>
@@ -1731,7 +1725,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7A54EA12-A463-48EB-8A81-36A2106B1F8B}" name="Factura3" displayName="Factura3" ref="B12:E23" totalsRowCount="1" headerRowDxfId="4" headerRowCellStyle="Encabezado 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7A54EA12-A463-48EB-8A81-36A2106B1F8B}" name="Factura3" displayName="Factura3" ref="B12:E23" totalsRowCount="1" headerRowDxfId="5" headerRowCellStyle="Encabezado 4">
   <autoFilter ref="B12:E22" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1740,9 +1734,9 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{965D0C2E-D7A3-43CD-BAD3-9FDE6883EEF5}" name="Cantidad"/>
-    <tableColumn id="2" xr3:uid="{92382F50-7070-433E-8576-EC3B54809EC6}" name="Descripción" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{92382F50-7070-433E-8576-EC3B54809EC6}" name="Descripción" totalsRowDxfId="4"/>
     <tableColumn id="4" xr3:uid="{C829CC40-5A68-4CAE-AA91-C1D1F3AB6B67}" name="Precio por unidad" totalsRowLabel="Subtotal"/>
-    <tableColumn id="5" xr3:uid="{76DF5326-18F6-4C6C-80D4-04BCF9259E7F}" name="Total de línea" totalsRowFunction="custom" totalsRowDxfId="2">
+    <tableColumn id="5" xr3:uid="{76DF5326-18F6-4C6C-80D4-04BCF9259E7F}" name="Total de línea" totalsRowFunction="custom" totalsRowDxfId="3">
       <calculatedColumnFormula>IFERROR(IF(SUM(B13)&gt;0,SUM(B13*D13),""), "")</calculatedColumnFormula>
       <totalsRowFormula>IFERROR(IF(SUM(E13:E22)&gt;0,SUM(E13:E22),""), "")</totalsRowFormula>
     </tableColumn>
@@ -1757,7 +1751,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Factura" displayName="Factura" ref="B13:E24" totalsRowCount="1" headerRowDxfId="5" headerRowCellStyle="Encabezado 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Factura" displayName="Factura" ref="B13:E24" totalsRowCount="1" headerRowDxfId="2" headerRowCellStyle="Encabezado 4">
   <autoFilter ref="B13:E23" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2066,7 +2060,7 @@
   </sheetPr>
   <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2084,14 +2078,14 @@
     <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="33"/>
+      <c r="D1" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2099,22 +2093,22 @@
     </row>
     <row r="3" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3">
         <v>45082</v>
@@ -2122,61 +2116,61 @@
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="41" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="41"/>
     </row>
     <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="40" t="s">
-        <v>38</v>
+      <c r="B8" s="36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="33" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" s="31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -2184,9 +2178,9 @@
         <v>1</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="37">
+        <v>24</v>
+      </c>
+      <c r="D13" s="33">
         <v>191.88</v>
       </c>
       <c r="E13" s="28">
@@ -2195,13 +2189,13 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="39">
+      <c r="B14" s="35">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="38">
+        <v>25</v>
+      </c>
+      <c r="D14" s="34">
         <v>20</v>
       </c>
       <c r="E14" s="28">
@@ -2214,9 +2208,9 @@
         <v>1</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="37">
+        <v>31</v>
+      </c>
+      <c r="D15" s="33">
         <v>11.95</v>
       </c>
       <c r="E15" s="28">
@@ -2225,13 +2219,13 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="39">
+      <c r="B16" s="35">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="38">
+        <v>26</v>
+      </c>
+      <c r="D16" s="34">
         <v>120</v>
       </c>
       <c r="E16" s="28">
@@ -2244,9 +2238,9 @@
         <v>1</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="37">
+        <v>27</v>
+      </c>
+      <c r="D17" s="33">
         <v>70</v>
       </c>
       <c r="E17" s="28">
@@ -2255,13 +2249,13 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39">
+      <c r="B18" s="35">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="38">
+        <v>28</v>
+      </c>
+      <c r="D18" s="34">
         <v>200</v>
       </c>
       <c r="E18" s="28">
@@ -2274,9 +2268,9 @@
         <v>1</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="37">
+        <v>29</v>
+      </c>
+      <c r="D19" s="33">
         <v>70</v>
       </c>
       <c r="E19" s="28">
@@ -2285,13 +2279,13 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="39">
+      <c r="B20" s="35">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="38">
+        <v>32</v>
+      </c>
+      <c r="D20" s="34">
         <v>1400</v>
       </c>
       <c r="E20" s="28">
@@ -2304,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="21">
@@ -2324,18 +2318,18 @@
     <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="23"/>
       <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="36">
+        <v>11</v>
+      </c>
+      <c r="E23" s="32">
         <f>IFERROR(IF(SUM(E13:E22)&gt;0,SUM(E13:E22),""), "")</f>
         <v>2083.83</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="34"/>
+      <c r="B24" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="38"/>
       <c r="D24" s="5">
         <v>0.21</v>
       </c>
@@ -2348,7 +2342,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E25" s="27">
         <f>IFERROR(IF(SUM(Factura3[[#Totals],[Total de línea]])&gt;0,SUM(Factura3[[#Totals],[Total de línea]],E24),""), "")</f>
@@ -2362,21 +2356,21 @@
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="35" t="str">
+      <c r="B27" s="39" t="str">
         <f>"Presupuesto válido durante 3 meses desde el envío de este documento."</f>
         <v>Presupuesto válido durante 3 meses desde el envío de este documento.</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
+      <c r="B28" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2424,7 +2418,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.51181102362204722" bottom="0.51181102362204722" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId3"/>
   <headerFooter differentFirst="1">
     <oddHeader>&amp;L&amp;G</oddHeader>
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
@@ -2448,15 +2442,15 @@
   </sheetPr>
   <dimension ref="B1:E29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="56.625" customWidth="1"/>
+    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="3" max="3" width="50.5" customWidth="1"/>
     <col min="4" max="4" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="18.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.625" customWidth="1"/>
@@ -2466,14 +2460,14 @@
     <row r="1" spans="2:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="33"/>
+      <c r="D1" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2481,22 +2475,22 @@
     </row>
     <row r="3" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3">
         <f ca="1">TODAY()</f>
@@ -2505,61 +2499,55 @@
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" s="31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -2567,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D14" s="28">
         <v>300</v>
@@ -2580,7 +2568,7 @@
     <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7" t="str">
@@ -2600,7 +2588,7 @@
     <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7" t="str">
@@ -2665,7 +2653,7 @@
     <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="23"/>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E24" s="25">
         <f>IFERROR(IF(SUM(E14:E23)&gt;0,SUM(E14:E23),""), "")</f>
@@ -2673,10 +2661,10 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="34"/>
+      <c r="B25" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="38"/>
       <c r="D25" s="5">
         <v>0.21</v>
       </c>
@@ -2689,7 +2677,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E26" s="27">
         <f>IFERROR(IF(SUM(Factura[[#Totals],[Total de línea]])&gt;0,SUM(Factura[[#Totals],[Total de línea]],E25),""), "")</f>
@@ -2703,21 +2691,21 @@
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="str">
+      <c r="B28" s="39" t="str">
         <f>"Presupuesto válido durante 3 meses desde el envío de este documento."</f>
         <v>Presupuesto válido durante 3 meses desde el envío de este documento.</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
+      <c r="B29" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2781,35 +2769,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3097,27 +3056,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{673FC2C4-7BD3-49D4-8830-2C75FF0E170D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEA9B86-3ACC-4F2F-B417-3306CFE473B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33998CD7-F07C-4773-9B85-057C9552A5A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3136,4 +3104,31 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEA9B86-3ACC-4F2F-B417-3306CFE473B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{673FC2C4-7BD3-49D4-8830-2C75FF0E170D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>